<commit_message>
Fixovanje problema sa povezivanjem
</commit_message>
<xml_diff>
--- a/backend/public/Izvestaj.xlsx
+++ b/backend/public/Izvestaj.xlsx
@@ -23,7 +23,7 @@
     <t>Datum</t>
   </si>
   <si>
-    <t>2022-06-16</t>
+    <t>2022-09-21</t>
   </si>
   <si>
     <t xml:space="preserve">Ukupan broj postova: </t>
@@ -32,7 +32,7 @@
     <t xml:space="preserve">Ukupan broj komentara: </t>
   </si>
   <si>
-    <t xml:space="preserve">Ukupan broj kafa: </t>
+    <t xml:space="preserve">Ukupan broj torti: </t>
   </si>
   <si>
     <t xml:space="preserve">Ukupan broj korinsika: </t>
@@ -47,7 +47,7 @@
     <t xml:space="preserve">Objava koja se najvise komentarise: </t>
   </si>
   <si>
-    <t>Naslov 1i</t>
+    <t>Čoko-lešnik torta (Novogodišnja torta)</t>
   </si>
 </sst>
 </file>
@@ -414,7 +414,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -422,7 +422,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -430,7 +430,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -438,7 +438,7 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -446,7 +446,7 @@
         <v>7</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -454,7 +454,7 @@
         <v>8</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:4">

</xml_diff>